<commit_message>
Disable this device answers to general calls
</commit_message>
<xml_diff>
--- a/timonel-testbed/test/Scope_Readings.xlsx
+++ b/timonel-testbed/test/Scope_Readings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casanovg\source\Repos\timonel\timonel-testbed\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825E4081-9218-4FC2-A6B2-FF5A07C4D56C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCFD32C-A86C-49E2-BCEF-7EB2DCD2667B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="1635" windowWidth="19065" windowHeight="7125" xr2:uid="{C45A570B-D4C0-4E00-B41F-5AC36C95DEC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C45A570B-D4C0-4E00-B41F-5AC36C95DEC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>